<commit_message>
remove delay when insert/remove safekey
</commit_message>
<xml_diff>
--- a/Audio/Audio.xlsx
+++ b/Audio/Audio.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RunningMachine\Audio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9847C8-D57F-4C9E-B3EC-EEC249165131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5510" yWindow="770" windowWidth="15360" windowHeight="15080"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -218,12 +219,18 @@
   <si>
     <t>Chào mừng bạn đến với máy tập thông minh Sport One.
 Hãy nhớ cài khóa an toàn trước khi luyện tập nhé. Nhấn phím start để chạy với tốc độ mặc định. Nhấn phím Stốp để dừng lại,hoặc quay trở lại cài đặt ban đầu. Nhấn và giữ Stốp 3 giây để tắt hoặc bật trợ lý ảo. Nhấn phím Program để lựa chọn các bài tập mặc định với độ dốc và tốc độ tự động thay đổi. Nhấn phím Mode để cài đặt thêm các thông số khác như thời gian,quãng đường,lượng calo tiêu thụ.</t>
+  </si>
+  <si>
+    <t>030</t>
+  </si>
+  <si>
+    <t>031</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -559,24 +566,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.453125" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.81640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31.26953125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" customWidth="1"/>
+    <col min="3" max="3" width="87.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +597,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -601,7 +608,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -612,7 +619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -623,7 +630,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -634,7 +641,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -645,7 +652,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -656,7 +663,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -667,7 +674,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -678,7 +685,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -689,7 +696,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -700,7 +707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -711,7 +718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -722,7 +729,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -733,7 +740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -744,7 +751,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -755,7 +762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -766,7 +773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -777,7 +784,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -788,7 +795,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -799,7 +806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -810,7 +817,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -821,7 +828,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -832,7 +839,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -843,7 +850,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -854,7 +861,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -865,7 +872,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -876,7 +883,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -887,7 +894,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -898,7 +905,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -909,106 +916,116 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="4"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="C31" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B32" s="4"/>
+    <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C32" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="3"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update code and audio theo comment cua chu Ha ngay 23/09
Chinh sua 1 vai file audio theo comment, sua code phan thoi gian chuc mung nguoi tap tu 20p thanh 5p
</commit_message>
<xml_diff>
--- a/Audio/Audio.xlsx
+++ b/Audio/Audio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\Audio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9847C8-D57F-4C9E-B3EC-EEC249165131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981333FB-4682-4CA6-BD93-BBF181E389F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>Bạn hãy cài khóa an toàn trước khi luyện tập nhé</t>
-  </si>
-  <si>
-    <t>Note</t>
   </si>
   <si>
     <t>027</t>
@@ -225,6 +222,45 @@
   </si>
   <si>
     <t>031</t>
+  </si>
+  <si>
+    <t>Cái này nói ngay khi khởi động</t>
+  </si>
+  <si>
+    <t>Chuyển sang 5 phút 1 lần</t>
+  </si>
+  <si>
+    <t>Bạn đã làm rất tốt, hãy rèn luyện chăm chỉ để có một cơ thể khỏe mạnh nhé</t>
+  </si>
+  <si>
+    <t>Bạn đã bắt đầu việc tập luyện, hãy chạy ở vận tốc này thêm một chút thời gian để khởi động và làm quen với máy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chào mừng bạn đến với máy tập thông minh Sport One.
+Bạn hãy dành 30 giây để nghe Huấn luyện viên Sport1 hướng dẫn cách sử dụng máy.Phím start để bắt đầu với tốc độ mặc định. Phím Stốp để dừng lại,hoặc quay trở lại cài đặt ban đầu.Nhấn và giữ Stốp 3 giây để tắt hoặc bật chế độ huấn luyện viên.Phím Program để chọn 1 trong 12 bài tập mặc định. Phím Mode để bạn tự thiết lập bài tập phù hợp. 
+(Nghỉ 1 nhip sau đó tiếp) Trước khi ấn nút Start để bắt đầu bạn nên đi giày và dành khoảng 10 phút để khởi động bằng các chức năng đã tích hợp trên máy như xoay eo,gập bụng và nhớ cài dây khóa an toàn trước khi tập. Nếu đã khởi động xong bạn hãy nhấn nút Start để bắt đầu.
+</t>
+  </si>
+  <si>
+    <t>Chúng ta tiếp tục luyện tập nhé</t>
+  </si>
+  <si>
+    <t>Chào mừng bạn đến với máy tập thông minh Sport One.
+Bạn hãy dành 30 giây để nghe Huấn luyện viên Sport1 hướng dẫn cách sử dụng máy.Phím start để bắt đầu với tốc độ mặc định. Phím Stốp để dừng lại,hoặc quay trở lại cài đặt ban đầu.Nhấn và giữ Stốp 3 giây để tắt hoặc bật chế độ huấn luyện viên.Phím Program để chọn 1 trong 12 bài tập mặc định. Phím Mode để bạn tự thiết lập bài tập phù hợp. 
+(Nghỉ 1 nhip sau đó tiếp) Trước khi ấn nút Start để bắt đầu bạn nên đi giày và dành khoảng 10 phút để khởi động bằng các chức năng đã tích hợp trên máy như xoay eo,gập bụng và nhớ cài dây khóa an toàn trước khi tập. Nếu đã khởi động xong bạn hãy nhấn nút Start để bắt đầu.</t>
+  </si>
+  <si>
+    <t>Bạn đã chạy được 2 phút với tốc độ và độ dốc hiện tại, để tăng cường độ tập bạn hãy bấm phím speed cộng để tăng hoặc speed trừ để giảm tốc độ, bấm phím mũi tên incline bên trái để tăng hoặc mũi tên incline bên phải để giảm độ dốc</t>
+  </si>
+  <si>
+    <t>Chuyển sang 1 phút
+Thống nhất lại là 2p</t>
+  </si>
+  <si>
+    <t>Note Change Code</t>
+  </si>
+  <si>
+    <t>Note 23/09 (Change audio)</t>
   </si>
 </sst>
 </file>
@@ -246,7 +282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +292,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,20 +326,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,466 +641,497 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="67.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="C28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B30" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B31" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>26</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>31</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>63</v>
+      <c r="D32" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
+      <c r="B34" s="5"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="4"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
+      <c r="B38" s="5"/>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="4"/>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
+      <c r="B40" s="5"/>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
+      <c r="B42" s="5"/>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
+      <c r="B44" s="5"/>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="4"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
+      <c r="B48" s="5"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
+      <c r="B50" s="5"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="4"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
+      <c r="B53" s="5"/>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="4"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="4"/>
+      <c r="B55" s="5"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
+      <c r="B57" s="5"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
+      <c r="B58" s="4"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
+      <c r="B59" s="4"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
+      <c r="B62" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>